<commit_message>
This should contains everything
</commit_message>
<xml_diff>
--- a/waypoints.xlsx
+++ b/waypoints.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgeEC9rFWnLYSd0csO9+2gInzdsBQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjKStULyERUJjwDJVdeo4F7w7SakQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="246">
   <si>
     <t>waypoint</t>
   </si>
@@ -72,15 +72,6 @@
     <t>:-544</t>
   </si>
   <si>
-    <t>:-1214</t>
-  </si>
-  <si>
-    <t>:19</t>
-  </si>
-  <si>
-    <t>:-512</t>
-  </si>
-  <si>
     <t>:-327</t>
   </si>
   <si>
@@ -267,279 +258,237 @@
     <t>:-306</t>
   </si>
   <si>
-    <t>:-1153</t>
-  </si>
-  <si>
-    <t>:51</t>
-  </si>
-  <si>
-    <t>:1144</t>
-  </si>
-  <si>
-    <t>:-260</t>
+    <t>:-343</t>
+  </si>
+  <si>
+    <t>:864</t>
+  </si>
+  <si>
+    <t>:796</t>
+  </si>
+  <si>
+    <t>:-213</t>
+  </si>
+  <si>
+    <t>:673</t>
+  </si>
+  <si>
+    <t>:38</t>
+  </si>
+  <si>
+    <t>:-374</t>
+  </si>
+  <si>
+    <t>:73</t>
+  </si>
+  <si>
+    <t>:32</t>
+  </si>
+  <si>
+    <t>:-441</t>
+  </si>
+  <si>
+    <t>:-939</t>
+  </si>
+  <si>
+    <t>:63</t>
+  </si>
+  <si>
+    <t>:454</t>
+  </si>
+  <si>
+    <t>:-701</t>
+  </si>
+  <si>
+    <t>:74</t>
+  </si>
+  <si>
+    <t>:1147</t>
+  </si>
+  <si>
+    <t>:-1065</t>
+  </si>
+  <si>
+    <t>:1477</t>
+  </si>
+  <si>
+    <t>:-1196</t>
+  </si>
+  <si>
+    <t>:65</t>
+  </si>
+  <si>
+    <t>:-89</t>
+  </si>
+  <si>
+    <t>:-329</t>
+  </si>
+  <si>
+    <t>:-1027</t>
   </si>
   <si>
     <t>:68</t>
   </si>
   <si>
-    <t>:1099</t>
-  </si>
-  <si>
-    <t>:-343</t>
-  </si>
-  <si>
-    <t>:864</t>
-  </si>
-  <si>
-    <t>:796</t>
-  </si>
-  <si>
-    <t>:-213</t>
-  </si>
-  <si>
-    <t>:673</t>
-  </si>
-  <si>
-    <t>:38</t>
-  </si>
-  <si>
-    <t>:-374</t>
-  </si>
-  <si>
-    <t>:-2159</t>
+    <t>:-75</t>
+  </si>
+  <si>
+    <t>:-1563</t>
+  </si>
+  <si>
+    <t>:10</t>
+  </si>
+  <si>
+    <t>:1472</t>
+  </si>
+  <si>
+    <t>:-1524</t>
+  </si>
+  <si>
+    <t>:8</t>
+  </si>
+  <si>
+    <t>:1244</t>
+  </si>
+  <si>
+    <t>:-2164</t>
+  </si>
+  <si>
+    <t>:783</t>
+  </si>
+  <si>
+    <t>:590</t>
+  </si>
+  <si>
+    <t>:882</t>
+  </si>
+  <si>
+    <t>:-595</t>
+  </si>
+  <si>
+    <t>:971</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>:-1966</t>
+  </si>
+  <si>
+    <t>:1198</t>
+  </si>
+  <si>
+    <t>:273</t>
+  </si>
+  <si>
+    <t>:61</t>
+  </si>
+  <si>
+    <t>:1560</t>
+  </si>
+  <si>
+    <t>:-1267</t>
+  </si>
+  <si>
+    <t>:-389</t>
+  </si>
+  <si>
+    <t>:-1969</t>
+  </si>
+  <si>
+    <t>:48</t>
+  </si>
+  <si>
+    <t>:1647</t>
+  </si>
+  <si>
+    <t>:269</t>
+  </si>
+  <si>
+    <t>:-269</t>
+  </si>
+  <si>
+    <t>:296</t>
+  </si>
+  <si>
+    <t>:-1606</t>
+  </si>
+  <si>
+    <t>:-355</t>
+  </si>
+  <si>
+    <t>:-1851</t>
+  </si>
+  <si>
+    <t>:82</t>
+  </si>
+  <si>
+    <t>:1387</t>
+  </si>
+  <si>
+    <t>:-1405</t>
+  </si>
+  <si>
+    <t>:53</t>
+  </si>
+  <si>
+    <t>:1103</t>
+  </si>
+  <si>
+    <t>:-1742</t>
+  </si>
+  <si>
+    <t>:67</t>
+  </si>
+  <si>
+    <t>:1648</t>
+  </si>
+  <si>
+    <t>:-744</t>
+  </si>
+  <si>
+    <t>:390</t>
+  </si>
+  <si>
+    <t>:1484</t>
+  </si>
+  <si>
+    <t>:-437</t>
+  </si>
+  <si>
+    <t>:6</t>
+  </si>
+  <si>
+    <t>:410</t>
+  </si>
+  <si>
+    <t>:-2132</t>
+  </si>
+  <si>
+    <t>:1790</t>
+  </si>
+  <si>
+    <t>:-1056</t>
+  </si>
+  <si>
+    <t>:-453</t>
+  </si>
+  <si>
+    <t>:-2010</t>
+  </si>
+  <si>
+    <t>:29</t>
+  </si>
+  <si>
+    <t>:-602</t>
+  </si>
+  <si>
+    <t>:-895</t>
   </si>
   <si>
     <t>:36</t>
   </si>
   <si>
-    <t>:-615</t>
-  </si>
-  <si>
-    <t>:73</t>
-  </si>
-  <si>
-    <t>:32</t>
-  </si>
-  <si>
-    <t>:-441</t>
-  </si>
-  <si>
-    <t>:-939</t>
-  </si>
-  <si>
-    <t>:63</t>
-  </si>
-  <si>
-    <t>:454</t>
-  </si>
-  <si>
-    <t>:-701</t>
-  </si>
-  <si>
-    <t>:74</t>
-  </si>
-  <si>
-    <t>:1147</t>
-  </si>
-  <si>
-    <t>:-1065</t>
-  </si>
-  <si>
-    <t>:1477</t>
-  </si>
-  <si>
-    <t>:-1196</t>
-  </si>
-  <si>
-    <t>:65</t>
-  </si>
-  <si>
-    <t>:-89</t>
-  </si>
-  <si>
-    <t>:-329</t>
-  </si>
-  <si>
-    <t>:-1027</t>
-  </si>
-  <si>
-    <t>:-75</t>
-  </si>
-  <si>
-    <t>:-713</t>
-  </si>
-  <si>
-    <t>:-171</t>
-  </si>
-  <si>
-    <t>:-1563</t>
-  </si>
-  <si>
-    <t>:10</t>
-  </si>
-  <si>
-    <t>:1472</t>
-  </si>
-  <si>
-    <t>:-1524</t>
-  </si>
-  <si>
-    <t>:8</t>
-  </si>
-  <si>
-    <t>:1244</t>
-  </si>
-  <si>
-    <t>:-2164</t>
-  </si>
-  <si>
-    <t>:783</t>
-  </si>
-  <si>
-    <t>:590</t>
-  </si>
-  <si>
-    <t>:882</t>
-  </si>
-  <si>
-    <t>:-595</t>
-  </si>
-  <si>
-    <t>:971</t>
-  </si>
-  <si>
-    <t>:-511</t>
-  </si>
-  <si>
-    <t>:53</t>
-  </si>
-  <si>
-    <t>:910</t>
-  </si>
-  <si>
-    <t>:-1966</t>
-  </si>
-  <si>
-    <t>:1198</t>
-  </si>
-  <si>
-    <t>:273</t>
-  </si>
-  <si>
-    <t>:61</t>
-  </si>
-  <si>
-    <t>:1560</t>
-  </si>
-  <si>
-    <t>:-1267</t>
-  </si>
-  <si>
-    <t>:-389</t>
-  </si>
-  <si>
-    <t>:-1969</t>
-  </si>
-  <si>
-    <t>:48</t>
-  </si>
-  <si>
-    <t>:1647</t>
-  </si>
-  <si>
-    <t>:-237</t>
-  </si>
-  <si>
-    <t>:56</t>
-  </si>
-  <si>
-    <t>:269</t>
-  </si>
-  <si>
-    <t>:-269</t>
-  </si>
-  <si>
-    <t>:296</t>
-  </si>
-  <si>
-    <t>:-1606</t>
-  </si>
-  <si>
-    <t>:-355</t>
-  </si>
-  <si>
-    <t>:-1851</t>
-  </si>
-  <si>
-    <t>:82</t>
-  </si>
-  <si>
-    <t>:1387</t>
-  </si>
-  <si>
-    <t>:-789</t>
-  </si>
-  <si>
-    <t>:30</t>
-  </si>
-  <si>
-    <t>:-1405</t>
-  </si>
-  <si>
-    <t>:1103</t>
-  </si>
-  <si>
-    <t>:-1742</t>
-  </si>
-  <si>
-    <t>:67</t>
-  </si>
-  <si>
-    <t>:1648</t>
-  </si>
-  <si>
-    <t>:-744</t>
-  </si>
-  <si>
-    <t>:390</t>
-  </si>
-  <si>
-    <t>:1484</t>
-  </si>
-  <si>
-    <t>:-437</t>
-  </si>
-  <si>
-    <t>:6</t>
-  </si>
-  <si>
-    <t>:410</t>
-  </si>
-  <si>
-    <t>:-2132</t>
-  </si>
-  <si>
-    <t>:1790</t>
-  </si>
-  <si>
-    <t>:-1056</t>
-  </si>
-  <si>
-    <t>:-453</t>
-  </si>
-  <si>
-    <t>:-2010</t>
-  </si>
-  <si>
-    <t>:29</t>
-  </si>
-  <si>
-    <t>:-602</t>
-  </si>
-  <si>
-    <t>:-895</t>
-  </si>
-  <si>
     <t>:54</t>
   </si>
   <si>
@@ -567,175 +516,166 @@
     <t>:1214</t>
   </si>
   <si>
+    <t>:264</t>
+  </si>
+  <si>
+    <t>:5</t>
+  </si>
+  <si>
+    <t>:1504</t>
+  </si>
+  <si>
+    <t>:598</t>
+  </si>
+  <si>
+    <t>:1132</t>
+  </si>
+  <si>
+    <t>:816</t>
+  </si>
+  <si>
+    <t>:931</t>
+  </si>
+  <si>
+    <t>:-364</t>
+  </si>
+  <si>
+    <t>:-55</t>
+  </si>
+  <si>
+    <t>:-2151</t>
+  </si>
+  <si>
+    <t>:1061</t>
+  </si>
+  <si>
+    <t>:457</t>
+  </si>
+  <si>
+    <t>:1440</t>
+  </si>
+  <si>
+    <t>:-1771</t>
+  </si>
+  <si>
+    <t>:1497</t>
+  </si>
+  <si>
+    <t>:-2097</t>
+  </si>
+  <si>
+    <t>:-143</t>
+  </si>
+  <si>
+    <t>:-1038</t>
+  </si>
+  <si>
+    <t>:1028</t>
+  </si>
+  <si>
+    <t>:-1021</t>
+  </si>
+  <si>
+    <t>:198</t>
+  </si>
+  <si>
+    <t>:80</t>
+  </si>
+  <si>
+    <t>:60</t>
+  </si>
+  <si>
+    <t>:1399</t>
+  </si>
+  <si>
+    <t>:732</t>
+  </si>
+  <si>
+    <t>:1816</t>
+  </si>
+  <si>
+    <t>:-2031</t>
+  </si>
+  <si>
+    <t>:75</t>
+  </si>
+  <si>
+    <t>:449</t>
+  </si>
+  <si>
+    <t>:-770</t>
+  </si>
+  <si>
+    <t>:-381</t>
+  </si>
+  <si>
+    <t>:-735</t>
+  </si>
+  <si>
+    <t>:17</t>
+  </si>
+  <si>
+    <t>:-531</t>
+  </si>
+  <si>
+    <t>:750</t>
+  </si>
+  <si>
+    <t>:1554</t>
+  </si>
+  <si>
+    <t>:801</t>
+  </si>
+  <si>
+    <t>:-81</t>
+  </si>
+  <si>
+    <t>:-546</t>
+  </si>
+  <si>
+    <t>:-234</t>
+  </si>
+  <si>
+    <t>:-1757</t>
+  </si>
+  <si>
+    <t>:1156</t>
+  </si>
+  <si>
+    <t>:824</t>
+  </si>
+  <si>
+    <t>:376</t>
+  </si>
+  <si>
+    <t>:-508</t>
+  </si>
+  <si>
+    <t>:1628</t>
+  </si>
+  <si>
+    <t>:-755</t>
+  </si>
+  <si>
+    <t>:57</t>
+  </si>
+  <si>
+    <t>:1742</t>
+  </si>
+  <si>
+    <t>:765</t>
+  </si>
+  <si>
+    <t>:1318</t>
+  </si>
+  <si>
+    <t>:-1179</t>
+  </si>
+  <si>
+    <t>:1855</t>
+  </si>
+  <si>
     <t>:77</t>
-  </si>
-  <si>
-    <t>:1206</t>
-  </si>
-  <si>
-    <t>:264</t>
-  </si>
-  <si>
-    <t>:5</t>
-  </si>
-  <si>
-    <t>:1504</t>
-  </si>
-  <si>
-    <t>:598</t>
-  </si>
-  <si>
-    <t>:1132</t>
-  </si>
-  <si>
-    <t>:816</t>
-  </si>
-  <si>
-    <t>:931</t>
-  </si>
-  <si>
-    <t>:-364</t>
-  </si>
-  <si>
-    <t>:-55</t>
-  </si>
-  <si>
-    <t>:-2151</t>
-  </si>
-  <si>
-    <t>:1061</t>
-  </si>
-  <si>
-    <t>:457</t>
-  </si>
-  <si>
-    <t>:1440</t>
-  </si>
-  <si>
-    <t>:-1771</t>
-  </si>
-  <si>
-    <t>:1497</t>
-  </si>
-  <si>
-    <t>:-2097</t>
-  </si>
-  <si>
-    <t>:-143</t>
-  </si>
-  <si>
-    <t>:-1038</t>
-  </si>
-  <si>
-    <t>:1028</t>
-  </si>
-  <si>
-    <t>:-1021</t>
-  </si>
-  <si>
-    <t>:198</t>
-  </si>
-  <si>
-    <t>:80</t>
-  </si>
-  <si>
-    <t>:60</t>
-  </si>
-  <si>
-    <t>:1399</t>
-  </si>
-  <si>
-    <t>:732</t>
-  </si>
-  <si>
-    <t>:1816</t>
-  </si>
-  <si>
-    <t>:-2031</t>
-  </si>
-  <si>
-    <t>:75</t>
-  </si>
-  <si>
-    <t>:449</t>
-  </si>
-  <si>
-    <t>:-770</t>
-  </si>
-  <si>
-    <t>:-381</t>
-  </si>
-  <si>
-    <t>:-735</t>
-  </si>
-  <si>
-    <t>:17</t>
-  </si>
-  <si>
-    <t>:-531</t>
-  </si>
-  <si>
-    <t>:750</t>
-  </si>
-  <si>
-    <t>:1554</t>
-  </si>
-  <si>
-    <t>:801</t>
-  </si>
-  <si>
-    <t>:-81</t>
-  </si>
-  <si>
-    <t>:-546</t>
-  </si>
-  <si>
-    <t>:-234</t>
-  </si>
-  <si>
-    <t>:-1757</t>
-  </si>
-  <si>
-    <t>:1156</t>
-  </si>
-  <si>
-    <t>:824</t>
-  </si>
-  <si>
-    <t>:376</t>
-  </si>
-  <si>
-    <t>:-508</t>
-  </si>
-  <si>
-    <t>:1628</t>
-  </si>
-  <si>
-    <t>:-755</t>
-  </si>
-  <si>
-    <t>:57</t>
-  </si>
-  <si>
-    <t>:1742</t>
-  </si>
-  <si>
-    <t>:765</t>
-  </si>
-  <si>
-    <t>:1318</t>
-  </si>
-  <si>
-    <t>:-1179</t>
-  </si>
-  <si>
-    <t>:1855</t>
-  </si>
-  <si>
-    <t>:-1753</t>
-  </si>
-  <si>
-    <t>:-627</t>
   </si>
   <si>
     <t>:-243</t>
@@ -852,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -860,6 +800,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1709,7 +1652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="2" t="s">
         <v>0</v>
       </c>
@@ -1887,10 +1830,10 @@
         <v>63</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>6</v>
@@ -1925,13 +1868,13 @@
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>6</v>
@@ -1966,13 +1909,13 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>6</v>
@@ -2007,10 +1950,10 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>71</v>
@@ -2051,10 +1994,10 @@
         <v>72</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>6</v>
@@ -2089,10 +2032,10 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>76</v>
@@ -2174,10 +2117,10 @@
         <v>80</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>6</v>
@@ -2212,13 +2155,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>6</v>
@@ -2253,13 +2196,13 @@
         <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>6</v>
@@ -2294,13 +2237,13 @@
         <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>6</v>
@@ -2335,10 +2278,10 @@
         <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>92</v>
@@ -2420,10 +2363,10 @@
         <v>96</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>6</v>
@@ -2458,13 +2401,13 @@
         <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>6</v>
@@ -2499,13 +2442,13 @@
         <v>2</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>6</v>
@@ -2540,13 +2483,13 @@
         <v>2</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>6</v>
@@ -2581,13 +2524,13 @@
         <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>6</v>
@@ -2622,13 +2565,13 @@
         <v>2</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>6</v>
@@ -2663,13 +2606,13 @@
         <v>2</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>6</v>
@@ -2704,13 +2647,13 @@
         <v>2</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>6</v>
@@ -2745,37 +2688,40 @@
         <v>2</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N42" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
       <c r="B43" s="2" t="s">
         <v>0</v>
       </c>
@@ -2789,10 +2735,10 @@
         <v>118</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>6</v>
@@ -2827,13 +2773,13 @@
         <v>2</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>6</v>
@@ -2868,13 +2814,13 @@
         <v>2</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>6</v>
@@ -2909,10 +2855,10 @@
         <v>2</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>127</v>
@@ -2953,10 +2899,10 @@
         <v>128</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>6</v>
@@ -2991,13 +2937,13 @@
         <v>2</v>
       </c>
       <c r="E48" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>6</v>
@@ -3032,13 +2978,13 @@
         <v>2</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>6</v>
@@ -3073,13 +3019,13 @@
         <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>6</v>
@@ -3114,13 +3060,13 @@
         <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>6</v>
@@ -3155,13 +3101,13 @@
         <v>2</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>6</v>
@@ -3196,13 +3142,13 @@
         <v>2</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>6</v>
@@ -3237,13 +3183,13 @@
         <v>2</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>145</v>
+        <v>9</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>6</v>
@@ -3278,10 +3224,10 @@
         <v>2</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>147</v>
@@ -3322,7 +3268,7 @@
         <v>148</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>149</v>
@@ -3363,10 +3309,10 @@
         <v>150</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>6</v>
@@ -3401,13 +3347,13 @@
         <v>2</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>6</v>
@@ -3445,10 +3391,10 @@
         <v>155</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>6</v>
@@ -3483,13 +3429,13 @@
         <v>2</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>6</v>
@@ -3524,13 +3470,13 @@
         <v>2</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>6</v>
@@ -3565,13 +3511,13 @@
         <v>2</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>6</v>
@@ -3606,13 +3552,13 @@
         <v>2</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>6</v>
@@ -3647,13 +3593,13 @@
         <v>2</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>43</v>
+        <v>159</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>6</v>
@@ -3688,13 +3634,13 @@
         <v>2</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>6</v>
@@ -3729,13 +3675,13 @@
         <v>2</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>171</v>
+        <v>49</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>6</v>
@@ -3770,13 +3716,13 @@
         <v>2</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>6</v>
@@ -3811,13 +3757,13 @@
         <v>2</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>176</v>
+        <v>52</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>6</v>
@@ -3852,10 +3798,10 @@
         <v>2</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>179</v>
+        <v>28</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>180</v>
@@ -3896,7 +3842,7 @@
         <v>181</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>182</v>
@@ -3937,7 +3883,7 @@
         <v>183</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>184</v>
@@ -3978,10 +3924,10 @@
         <v>185</v>
       </c>
       <c r="F72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>6</v>
@@ -4016,10 +3962,10 @@
         <v>2</v>
       </c>
       <c r="E73" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>189</v>
@@ -4060,7 +4006,7 @@
         <v>190</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>191</v>
@@ -4101,10 +4047,10 @@
         <v>192</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>52</v>
+        <v>193</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>6</v>
@@ -4139,13 +4085,13 @@
         <v>2</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>43</v>
+        <v>159</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>6</v>
@@ -4180,13 +4126,13 @@
         <v>2</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>55</v>
+        <v>198</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>6</v>
@@ -4221,13 +4167,13 @@
         <v>2</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>31</v>
+        <v>193</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>6</v>
@@ -4262,13 +4208,13 @@
         <v>2</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>6</v>
@@ -4303,13 +4249,13 @@
         <v>2</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>6</v>
@@ -4344,13 +4290,13 @@
         <v>2</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>6</v>
@@ -4385,13 +4331,13 @@
         <v>2</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>207</v>
+        <v>37</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>6</v>
@@ -4426,13 +4372,13 @@
         <v>2</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>6</v>
@@ -4467,13 +4413,13 @@
         <v>2</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>6</v>
@@ -4508,13 +4454,13 @@
         <v>2</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>6</v>
@@ -4549,10 +4495,10 @@
         <v>2</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>217</v>
+        <v>94</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>218</v>
@@ -4590,13 +4536,13 @@
         <v>2</v>
       </c>
       <c r="E87" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="G87" s="1" t="s">
-        <v>220</v>
+        <v>141</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>6</v>
@@ -4631,13 +4577,13 @@
         <v>2</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>221</v>
+        <v>78</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>6</v>
@@ -4672,13 +4618,13 @@
         <v>2</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>176</v>
+        <v>31</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>6</v>
@@ -4713,13 +4659,13 @@
         <v>2</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>6</v>
@@ -4754,13 +4700,13 @@
         <v>2</v>
       </c>
       <c r="E91" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G91" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>6</v>
@@ -4795,13 +4741,13 @@
         <v>2</v>
       </c>
       <c r="E92" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G92" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>6</v>
@@ -4836,13 +4782,13 @@
         <v>2</v>
       </c>
       <c r="E93" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G93" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>6</v>
@@ -4877,13 +4823,13 @@
         <v>2</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>179</v>
+        <v>94</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>6</v>
@@ -4918,13 +4864,13 @@
         <v>2</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>106</v>
+        <v>193</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>6</v>
@@ -4959,13 +4905,13 @@
         <v>2</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>6</v>
@@ -5000,13 +4946,13 @@
         <v>2</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>34</v>
+        <v>238</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>159</v>
+        <v>239</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>6</v>
@@ -5041,13 +4987,13 @@
         <v>2</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>81</v>
+        <v>240</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>6</v>
@@ -5082,13 +5028,13 @@
         <v>2</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>6</v>
@@ -5123,13 +5069,13 @@
         <v>2</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>6</v>
@@ -5154,414 +5100,54 @@
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="B101" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L101" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M101" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N101" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="B102" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="H102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K102" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L102" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N102" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="B103" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L103" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N103" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="B104" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L104" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N104" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="B105" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="H105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I105" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K105" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L105" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N105" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="B106" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K106" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L106" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N106" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="B107" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K107" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L107" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N107" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="B108" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K108" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L108" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N108" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="B109" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="H109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K109" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L109" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N109" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="B110" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I110" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K110" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L110" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N110" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="E111" s="1"/>
@@ -9882,56 +9468,6 @@
       <c r="E974" s="1"/>
       <c r="F974" s="1"/>
       <c r="G974" s="1"/>
-    </row>
-    <row r="975" ht="15.75" customHeight="1">
-      <c r="E975" s="1"/>
-      <c r="F975" s="1"/>
-      <c r="G975" s="1"/>
-    </row>
-    <row r="976" ht="15.75" customHeight="1">
-      <c r="E976" s="1"/>
-      <c r="F976" s="1"/>
-      <c r="G976" s="1"/>
-    </row>
-    <row r="977" ht="15.75" customHeight="1">
-      <c r="E977" s="1"/>
-      <c r="F977" s="1"/>
-      <c r="G977" s="1"/>
-    </row>
-    <row r="978" ht="15.75" customHeight="1">
-      <c r="E978" s="1"/>
-      <c r="F978" s="1"/>
-      <c r="G978" s="1"/>
-    </row>
-    <row r="979" ht="15.75" customHeight="1">
-      <c r="E979" s="1"/>
-      <c r="F979" s="1"/>
-      <c r="G979" s="1"/>
-    </row>
-    <row r="980" ht="15.75" customHeight="1">
-      <c r="E980" s="1"/>
-      <c r="F980" s="1"/>
-      <c r="G980" s="1"/>
-    </row>
-    <row r="981" ht="15.75" customHeight="1">
-      <c r="E981" s="1"/>
-      <c r="F981" s="1"/>
-      <c r="G981" s="1"/>
-    </row>
-    <row r="982" ht="15.75" customHeight="1">
-      <c r="E982" s="1"/>
-      <c r="F982" s="1"/>
-      <c r="G982" s="1"/>
-    </row>
-    <row r="983" ht="15.75" customHeight="1">
-      <c r="E983" s="1"/>
-      <c r="F983" s="1"/>
-      <c r="G983" s="1"/>
-    </row>
-    <row r="984" ht="15.75" customHeight="1">
-      <c r="E984" s="1"/>
-      <c r="F984" s="1"/>
-      <c r="G984" s="1"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>